<commit_message>
Updating Voila app to use S5
</commit_message>
<xml_diff>
--- a/Norway_Morsa/MetData_Processing/notebooks/07_s5_download_combos.xlsx
+++ b/Norway_Morsa/MetData_Processing/notebooks/07_s5_download_combos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815684CF-1ECD-4EE6-878F-DE4F3F164FEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E963B48-0953-4A7E-8E75-14D95CB0E166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4867" yWindow="1163" windowWidth="21315" windowHeight="12397" xr2:uid="{95BBEEF8-4457-42DC-82CF-991EAA9544AB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{95BBEEF8-4457-42DC-82CF-991EAA9544AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="35">
   <si>
     <t>period</t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>2,3,4</t>
+  </si>
+  <si>
+    <t>early_summer</t>
+  </si>
+  <si>
+    <t>5,6,7</t>
+  </si>
+  <si>
+    <t>8,9,10</t>
+  </si>
+  <si>
+    <t>Added 10.03.2020</t>
   </si>
 </sst>
 </file>
@@ -176,12 +188,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE07BAA-510C-4C30-A0C4-158DEE824910}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -507,11 +520,11 @@
     <col min="1" max="1" width="8.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.9296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.86328125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.33203125" customWidth="1"/>
+    <col min="8" max="8" width="39.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
@@ -924,6 +937,214 @@
       </c>
       <c r="H17" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>